<commit_message>
Clean code and explanations
</commit_message>
<xml_diff>
--- a/database/simplerealnodes.xlsx
+++ b/database/simplerealnodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomasodeponti/Desktop/C&amp;S/Q1/Operations optimisation/project/gurobi trial/AE4441-Group-2-VRP-Project/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BB0E99-00BC-7F42-8635-2B2D0A8CAB3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95302FD6-29F6-2E4C-91E0-842A41ADE17A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="16020" xr2:uid="{FCBBAB21-A819-C842-AE39-F68DB9AAE298}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>From</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Distance</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -416,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21B481E-55ED-444F-A9EF-284BDD615991}">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +437,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -445,8 +451,11 @@
       <c r="C2">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" cm="1">
         <f t="array" ref="A3">IF(MOD(ROW(2:2)-1,9)=0,A2+1,A2)</f>
         <v>1</v>
@@ -458,8 +467,11 @@
       <c r="C3">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" cm="1">
         <f t="array" ref="A4">IF(MOD(ROW(3:3)-1,9)=0,A3+1,A3)</f>
         <v>1</v>
@@ -471,8 +483,11 @@
       <c r="C4">
         <v>226</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" cm="1">
         <f t="array" ref="A5">IF(MOD(ROW(4:4)-1,9)=0,A4+1,A4)</f>
         <v>1</v>
@@ -484,8 +499,11 @@
       <c r="C5">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" cm="1">
         <f t="array" ref="A6">IF(MOD(ROW(5:5)-1,9)=0,A5+1,A5)</f>
         <v>1</v>
@@ -497,8 +515,11 @@
       <c r="C6">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" cm="1">
         <f t="array" ref="A7">IF(MOD(ROW(6:6)-1,9)=0,A6+1,A6)</f>
         <v>1</v>
@@ -510,8 +531,11 @@
       <c r="C7">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" cm="1">
         <f t="array" ref="A8">IF(MOD(ROW(7:7)-1,9)=0,A7+1,A7)</f>
         <v>1</v>
@@ -523,8 +547,11 @@
       <c r="C8">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" cm="1">
         <f t="array" ref="A9">IF(MOD(ROW(8:8)-1,9)=0,A8+1,A8)</f>
         <v>1</v>
@@ -536,8 +563,11 @@
       <c r="C9">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" cm="1">
         <f t="array" ref="A10">IF(MOD(ROW(9:9)-1,9)=0,A9+1,A9)</f>
         <v>1</v>
@@ -549,8 +579,11 @@
       <c r="C10">
         <v>125</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" cm="1">
         <f t="array" ref="A11">IF(MOD(ROW(10:10)-1,9)=0,A10+1,A10)</f>
         <v>2</v>
@@ -562,8 +595,11 @@
       <c r="C11">
         <v>97</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" cm="1">
         <f t="array" ref="A12">IF(MOD(ROW(11:11)-1,9)=0,A11+1,A11)</f>
         <v>2</v>
@@ -575,8 +611,11 @@
       <c r="C12">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" cm="1">
         <f t="array" ref="A13">IF(MOD(ROW(12:12)-1,9)=0,A12+1,A12)</f>
         <v>2</v>
@@ -588,8 +627,11 @@
       <c r="C13">
         <v>153</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" cm="1">
         <f t="array" ref="A14">IF(MOD(ROW(13:13)-1,9)=0,A13+1,A13)</f>
         <v>2</v>
@@ -601,8 +643,11 @@
       <c r="C14">
         <v>157</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" cm="1">
         <f t="array" ref="A15">IF(MOD(ROW(14:14)-1,9)=0,A14+1,A14)</f>
         <v>2</v>
@@ -614,8 +659,11 @@
       <c r="C15">
         <v>131</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" cm="1">
         <f t="array" ref="A16">IF(MOD(ROW(15:15)-1,9)=0,A15+1,A15)</f>
         <v>2</v>
@@ -627,8 +675,11 @@
       <c r="C16">
         <v>115</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" cm="1">
         <f t="array" ref="A17">IF(MOD(ROW(16:16)-1,9)=0,A16+1,A16)</f>
         <v>2</v>
@@ -640,8 +691,11 @@
       <c r="C17">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" cm="1">
         <f t="array" ref="A18">IF(MOD(ROW(17:17)-1,9)=0,A17+1,A17)</f>
         <v>2</v>
@@ -653,8 +707,11 @@
       <c r="C18">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" cm="1">
         <f t="array" ref="A19">IF(MOD(ROW(18:18)-1,9)=0,A18+1,A18)</f>
         <v>2</v>
@@ -666,8 +723,11 @@
       <c r="C19">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" cm="1">
         <f t="array" ref="A20">IF(MOD(ROW(19:19)-1,9)=0,A19+1,A19)</f>
         <v>3</v>
@@ -679,8 +739,11 @@
       <c r="C20">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" cm="1">
         <f t="array" ref="A21">IF(MOD(ROW(20:20)-1,9)=0,A20+1,A20)</f>
         <v>3</v>
@@ -692,8 +755,11 @@
       <c r="C21">
         <v>84</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" cm="1">
         <f t="array" ref="A22">IF(MOD(ROW(21:21)-1,9)=0,A21+1,A21)</f>
         <v>3</v>
@@ -705,8 +771,11 @@
       <c r="C22">
         <v>134</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" cm="1">
         <f t="array" ref="A23">IF(MOD(ROW(22:22)-1,9)=0,A22+1,A22)</f>
         <v>3</v>
@@ -718,8 +787,11 @@
       <c r="C23">
         <v>146</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" cm="1">
         <f t="array" ref="A24">IF(MOD(ROW(23:23)-1,9)=0,A23+1,A23)</f>
         <v>3</v>
@@ -731,8 +803,11 @@
       <c r="C24">
         <v>154</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" cm="1">
         <f t="array" ref="A25">IF(MOD(ROW(24:24)-1,9)=0,A24+1,A24)</f>
         <v>3</v>
@@ -744,8 +819,11 @@
       <c r="C25">
         <v>120</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" cm="1">
         <f t="array" ref="A26">IF(MOD(ROW(25:25)-1,9)=0,A25+1,A25)</f>
         <v>3</v>
@@ -757,8 +835,11 @@
       <c r="C26">
         <v>107</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" cm="1">
         <f t="array" ref="A27">IF(MOD(ROW(26:26)-1,9)=0,A26+1,A26)</f>
         <v>3</v>
@@ -770,8 +851,11 @@
       <c r="C27">
         <v>114</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" cm="1">
         <f t="array" ref="A28">IF(MOD(ROW(27:27)-1,9)=0,A27+1,A27)</f>
         <v>3</v>
@@ -783,8 +867,11 @@
       <c r="C28">
         <v>137</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" cm="1">
         <f t="array" ref="A29">IF(MOD(ROW(28:28)-1,9)=0,A28+1,A28)</f>
         <v>4</v>
@@ -796,8 +883,11 @@
       <c r="C29">
         <v>226</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" cm="1">
         <f t="array" ref="A30">IF(MOD(ROW(29:29)-1,9)=0,A29+1,A29)</f>
         <v>4</v>
@@ -809,8 +899,11 @@
       <c r="C30">
         <v>153</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" cm="1">
         <f t="array" ref="A31">IF(MOD(ROW(30:30)-1,9)=0,A30+1,A30)</f>
         <v>4</v>
@@ -822,8 +915,11 @@
       <c r="C31">
         <v>134</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" cm="1">
         <f t="array" ref="A32">IF(MOD(ROW(31:31)-1,9)=0,A31+1,A31)</f>
         <v>4</v>
@@ -835,8 +931,11 @@
       <c r="C32">
         <v>279</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" cm="1">
         <f t="array" ref="A33">IF(MOD(ROW(32:32)-1,9)=0,A32+1,A32)</f>
         <v>4</v>
@@ -848,8 +947,11 @@
       <c r="C33">
         <v>274</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" cm="1">
         <f t="array" ref="A34">IF(MOD(ROW(33:33)-1,9)=0,A33+1,A33)</f>
         <v>4</v>
@@ -861,8 +963,11 @@
       <c r="C34">
         <v>247</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" cm="1">
         <f t="array" ref="A35">IF(MOD(ROW(34:34)-1,9)=0,A34+1,A34)</f>
         <v>4</v>
@@ -874,8 +979,11 @@
       <c r="C35">
         <v>223</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" cm="1">
         <f t="array" ref="A36">IF(MOD(ROW(35:35)-1,9)=0,A35+1,A35)</f>
         <v>4</v>
@@ -887,8 +995,11 @@
       <c r="C36">
         <v>209</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" cm="1">
         <f t="array" ref="A37">IF(MOD(ROW(36:36)-1,9)=0,A36+1,A36)</f>
         <v>4</v>
@@ -900,8 +1011,11 @@
       <c r="C37">
         <v>188</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" cm="1">
         <f t="array" ref="A38">IF(MOD(ROW(37:37)-1,9)=0,A37+1,A37)</f>
         <v>5</v>
@@ -913,8 +1027,11 @@
       <c r="C38">
         <v>60</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" cm="1">
         <f t="array" ref="A39">IF(MOD(ROW(38:38)-1,9)=0,A38+1,A38)</f>
         <v>5</v>
@@ -926,8 +1043,11 @@
       <c r="C39">
         <v>157</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" cm="1">
         <f t="array" ref="A40">IF(MOD(ROW(39:39)-1,9)=0,A39+1,A39)</f>
         <v>5</v>
@@ -939,8 +1059,11 @@
       <c r="C40">
         <v>146</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" cm="1">
         <f t="array" ref="A41">IF(MOD(ROW(40:40)-1,9)=0,A40+1,A40)</f>
         <v>5</v>
@@ -952,8 +1075,11 @@
       <c r="C41">
         <v>279</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" cm="1">
         <f t="array" ref="A42">IF(MOD(ROW(41:41)-1,9)=0,A41+1,A41)</f>
         <v>5</v>
@@ -965,8 +1091,11 @@
       <c r="C42">
         <v>61</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" cm="1">
         <f t="array" ref="A43">IF(MOD(ROW(42:42)-1,9)=0,A42+1,A42)</f>
         <v>5</v>
@@ -978,8 +1107,11 @@
       <c r="C43">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" cm="1">
         <f t="array" ref="A44">IF(MOD(ROW(43:43)-1,9)=0,A43+1,A43)</f>
         <v>5</v>
@@ -991,8 +1123,11 @@
       <c r="C44">
         <v>80</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" cm="1">
         <f t="array" ref="A45">IF(MOD(ROW(44:44)-1,9)=0,A44+1,A44)</f>
         <v>5</v>
@@ -1004,8 +1139,11 @@
       <c r="C45">
         <v>119</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" cm="1">
         <f t="array" ref="A46">IF(MOD(ROW(45:45)-1,9)=0,A45+1,A45)</f>
         <v>5</v>
@@ -1017,8 +1155,11 @@
       <c r="C46">
         <v>181</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" cm="1">
         <f t="array" ref="A47">IF(MOD(ROW(46:46)-1,9)=0,A46+1,A46)</f>
         <v>6</v>
@@ -1030,8 +1171,11 @@
       <c r="C47">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" cm="1">
         <f t="array" ref="A48">IF(MOD(ROW(47:47)-1,9)=0,A47+1,A47)</f>
         <v>6</v>
@@ -1043,8 +1187,11 @@
       <c r="C48">
         <v>131</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" cm="1">
         <f t="array" ref="A49">IF(MOD(ROW(48:48)-1,9)=0,A48+1,A48)</f>
         <v>6</v>
@@ -1056,8 +1203,11 @@
       <c r="C49">
         <v>154</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" cm="1">
         <f t="array" ref="A50">IF(MOD(ROW(49:49)-1,9)=0,A49+1,A49)</f>
         <v>6</v>
@@ -1069,8 +1219,11 @@
       <c r="C50">
         <v>274</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" cm="1">
         <f t="array" ref="A51">IF(MOD(ROW(50:50)-1,9)=0,A50+1,A50)</f>
         <v>6</v>
@@ -1082,8 +1235,11 @@
       <c r="C51">
         <v>61</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" cm="1">
         <f t="array" ref="A52">IF(MOD(ROW(51:51)-1,9)=0,A51+1,A51)</f>
         <v>6</v>
@@ -1095,8 +1251,11 @@
       <c r="C52">
         <v>38</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" cm="1">
         <f t="array" ref="A53">IF(MOD(ROW(52:52)-1,9)=0,A52+1,A52)</f>
         <v>6</v>
@@ -1108,8 +1267,11 @@
       <c r="C53">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" cm="1">
         <f t="array" ref="A54">IF(MOD(ROW(53:53)-1,9)=0,A53+1,A53)</f>
         <v>6</v>
@@ -1121,8 +1283,11 @@
       <c r="C54">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" cm="1">
         <f t="array" ref="A55">IF(MOD(ROW(54:54)-1,9)=0,A54+1,A54)</f>
         <v>6</v>
@@ -1134,8 +1299,11 @@
       <c r="C55">
         <v>138</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" cm="1">
         <f t="array" ref="A56">IF(MOD(ROW(55:55)-1,9)=0,A55+1,A55)</f>
         <v>7</v>
@@ -1147,8 +1315,11 @@
       <c r="C56">
         <v>21</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" cm="1">
         <f t="array" ref="A57">IF(MOD(ROW(56:56)-1,9)=0,A56+1,A56)</f>
         <v>7</v>
@@ -1160,8 +1331,11 @@
       <c r="C57">
         <v>115</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" cm="1">
         <f t="array" ref="A58">IF(MOD(ROW(57:57)-1,9)=0,A57+1,A57)</f>
         <v>7</v>
@@ -1173,8 +1347,11 @@
       <c r="C58">
         <v>120</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" cm="1">
         <f t="array" ref="A59">IF(MOD(ROW(58:58)-1,9)=0,A58+1,A58)</f>
         <v>7</v>
@@ -1186,8 +1363,11 @@
       <c r="C59">
         <v>247</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" cm="1">
         <f t="array" ref="A60">IF(MOD(ROW(59:59)-1,9)=0,A59+1,A59)</f>
         <v>7</v>
@@ -1199,8 +1379,11 @@
       <c r="C60">
         <v>44</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" cm="1">
         <f t="array" ref="A61">IF(MOD(ROW(60:60)-1,9)=0,A60+1,A60)</f>
         <v>7</v>
@@ -1212,8 +1395,11 @@
       <c r="C61">
         <v>38</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" cm="1">
         <f t="array" ref="A62">IF(MOD(ROW(61:61)-1,9)=0,A61+1,A61)</f>
         <v>7</v>
@@ -1225,8 +1411,11 @@
       <c r="C62">
         <v>36</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" cm="1">
         <f t="array" ref="A63">IF(MOD(ROW(62:62)-1,9)=0,A62+1,A62)</f>
         <v>7</v>
@@ -1238,8 +1427,11 @@
       <c r="C63">
         <v>75</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" cm="1">
         <f t="array" ref="A64">IF(MOD(ROW(63:63)-1,9)=0,A63+1,A63)</f>
         <v>7</v>
@@ -1251,8 +1443,11 @@
       <c r="C64">
         <v>137</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" cm="1">
         <f t="array" ref="A65">IF(MOD(ROW(64:64)-1,9)=0,A64+1,A64)</f>
         <v>8</v>
@@ -1264,8 +1459,11 @@
       <c r="C65">
         <v>27</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" cm="1">
         <f t="array" ref="A66">IF(MOD(ROW(65:65)-1,9)=0,A65+1,A65)</f>
         <v>8</v>
@@ -1277,8 +1475,11 @@
       <c r="C66">
         <v>82</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" cm="1">
         <f t="array" ref="A67">IF(MOD(ROW(66:66)-1,9)=0,A66+1,A66)</f>
         <v>8</v>
@@ -1290,8 +1491,11 @@
       <c r="C67">
         <v>107</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" cm="1">
         <f t="array" ref="A68">IF(MOD(ROW(67:67)-1,9)=0,A67+1,A67)</f>
         <v>8</v>
@@ -1303,8 +1507,11 @@
       <c r="C68">
         <v>223</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" cm="1">
         <f t="array" ref="A69">IF(MOD(ROW(68:68)-1,9)=0,A68+1,A68)</f>
         <v>8</v>
@@ -1316,8 +1523,11 @@
       <c r="C69">
         <v>80</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" cm="1">
         <f t="array" ref="A70">IF(MOD(ROW(69:69)-1,9)=0,A69+1,A69)</f>
         <v>8</v>
@@ -1329,8 +1539,11 @@
       <c r="C70">
         <v>51</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" cm="1">
         <f t="array" ref="A71">IF(MOD(ROW(70:70)-1,9)=0,A70+1,A70)</f>
         <v>8</v>
@@ -1342,8 +1555,11 @@
       <c r="C71">
         <v>36</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" cm="1">
         <f t="array" ref="A72">IF(MOD(ROW(71:71)-1,9)=0,A71+1,A71)</f>
         <v>8</v>
@@ -1355,8 +1571,11 @@
       <c r="C72">
         <v>39</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" cm="1">
         <f t="array" ref="A73">IF(MOD(ROW(72:72)-1,9)=0,A72+1,A72)</f>
         <v>8</v>
@@ -1368,8 +1587,11 @@
       <c r="C73">
         <v>101</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" cm="1">
         <f t="array" ref="A74">IF(MOD(ROW(73:73)-1,9)=0,A73+1,A73)</f>
         <v>9</v>
@@ -1381,8 +1603,11 @@
       <c r="C74">
         <v>66</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" cm="1">
         <f t="array" ref="A75">IF(MOD(ROW(74:74)-1,9)=0,A74+1,A74)</f>
         <v>9</v>
@@ -1394,8 +1619,11 @@
       <c r="C75">
         <v>57</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" cm="1">
         <f t="array" ref="A76">IF(MOD(ROW(75:75)-1,9)=0,A75+1,A75)</f>
         <v>9</v>
@@ -1407,8 +1635,11 @@
       <c r="C76">
         <v>114</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" cm="1">
         <f t="array" ref="A77">IF(MOD(ROW(76:76)-1,9)=0,A76+1,A76)</f>
         <v>9</v>
@@ -1420,8 +1651,11 @@
       <c r="C77">
         <v>209</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" cm="1">
         <f t="array" ref="A78">IF(MOD(ROW(77:77)-1,9)=0,A77+1,A77)</f>
         <v>9</v>
@@ -1433,8 +1667,11 @@
       <c r="C78">
         <v>119</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" cm="1">
         <f t="array" ref="A79">IF(MOD(ROW(78:78)-1,9)=0,A78+1,A78)</f>
         <v>9</v>
@@ -1446,8 +1683,11 @@
       <c r="C79">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" cm="1">
         <f t="array" ref="A80">IF(MOD(ROW(79:79)-1,9)=0,A79+1,A79)</f>
         <v>9</v>
@@ -1459,8 +1699,11 @@
       <c r="C80">
         <v>75</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" cm="1">
         <f t="array" ref="A81">IF(MOD(ROW(80:80)-1,9)=0,A80+1,A80)</f>
         <v>9</v>
@@ -1472,8 +1715,11 @@
       <c r="C81">
         <v>39</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" cm="1">
         <f t="array" ref="A82">IF(MOD(ROW(81:81)-1,9)=0,A81+1,A81)</f>
         <v>9</v>
@@ -1485,8 +1731,11 @@
       <c r="C82">
         <v>62</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" cm="1">
         <f t="array" ref="A83">IF(MOD(ROW(82:82)-1,9)=0,A82+1,A82)</f>
         <v>10</v>
@@ -1498,8 +1747,11 @@
       <c r="C83">
         <v>125</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" cm="1">
         <f t="array" ref="A84">IF(MOD(ROW(83:83)-1,9)=0,A83+1,A83)</f>
         <v>10</v>
@@ -1511,8 +1763,11 @@
       <c r="C84">
         <v>53</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" cm="1">
         <f t="array" ref="A85">IF(MOD(ROW(84:84)-1,9)=0,A84+1,A84)</f>
         <v>10</v>
@@ -1524,8 +1779,11 @@
       <c r="C85">
         <v>137</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" cm="1">
         <f t="array" ref="A86">IF(MOD(ROW(85:85)-1,9)=0,A85+1,A85)</f>
         <v>10</v>
@@ -1537,8 +1795,11 @@
       <c r="C86">
         <v>188</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" cm="1">
         <f t="array" ref="A87">IF(MOD(ROW(86:86)-1,9)=0,A86+1,A86)</f>
         <v>10</v>
@@ -1550,8 +1811,11 @@
       <c r="C87">
         <v>181</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" cm="1">
         <f t="array" ref="A88">IF(MOD(ROW(87:87)-1,9)=0,A87+1,A87)</f>
         <v>10</v>
@@ -1563,8 +1827,11 @@
       <c r="C88">
         <v>138</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" cm="1">
         <f t="array" ref="A89">IF(MOD(ROW(88:88)-1,9)=0,A88+1,A88)</f>
         <v>10</v>
@@ -1576,8 +1843,11 @@
       <c r="C89">
         <v>137</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" cm="1">
         <f t="array" ref="A90">IF(MOD(ROW(89:89)-1,9)=0,A89+1,A89)</f>
         <v>10</v>
@@ -1589,8 +1859,11 @@
       <c r="C90">
         <v>101</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" cm="1">
         <f t="array" ref="A91">IF(MOD(ROW(90:90)-1,9)=0,A90+1,A90)</f>
         <v>10</v>
@@ -1601,6 +1874,9 @@
       </c>
       <c r="C91">
         <v>62</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>